<commit_message>
Updated BI Monthly Project Status Report
Signed-off-by: Mohamed younus A <31933@Hexaware.com>
</commit_message>
<xml_diff>
--- a/BFS/CRES/MonthlyProjectStatusReport-CRES Offering_May2016.xlsx
+++ b/BFS/CRES/MonthlyProjectStatusReport-CRES Offering_May2016.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
   <si>
     <t>Project ID</t>
   </si>
@@ -55,54 +55,15 @@
     <t>Training Needs</t>
   </si>
   <si>
-    <t>&lt;any training pending&gt;</t>
-  </si>
-  <si>
-    <t>&lt;mention the pending needs and challenges if any&gt;</t>
-  </si>
-  <si>
     <t>Critical Risks</t>
   </si>
   <si>
-    <t>&lt;Count of open risks&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Refer critical risks from PP&gt;</t>
-  </si>
-  <si>
     <t>Critical Issues</t>
   </si>
   <si>
-    <t>&lt;Count of open issues&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Refer critical issues from PP / WSR&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review by Competency </t>
-  </si>
-  <si>
     <t>&lt;Review conducted in reporting period&gt;</t>
   </si>
   <si>
-    <t>&lt;Plan for next month&gt;</t>
-  </si>
-  <si>
-    <t>PHI</t>
-  </si>
-  <si>
-    <t>Target &lt;&gt;, Actuals &lt;&gt;</t>
-  </si>
-  <si>
-    <t>Open NC / Observations of IQA</t>
-  </si>
-  <si>
-    <t>&lt;Count of NC&gt; and &lt;Audit Score&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Refer IQA Tool&gt;</t>
-  </si>
-  <si>
     <t>Project Execution</t>
   </si>
   <si>
@@ -151,9 +112,6 @@
     <t>Number of post shipment defects</t>
   </si>
   <si>
-    <t xml:space="preserve">Severity </t>
-  </si>
-  <si>
     <t>High &lt;count&gt;</t>
   </si>
   <si>
@@ -224,9 +182,6 @@
   </si>
   <si>
     <t>G7</t>
-  </si>
-  <si>
-    <t>Count of Grade</t>
   </si>
   <si>
     <t>Row Labels</t>
@@ -263,13 +218,142 @@
     <t>CRES Offering</t>
   </si>
   <si>
-    <t>CRES Service Offering is a solution to measure  the utilization of seats, meeting room and board room facilities in percentage. 
+    <t>PRJ-4660 - OEG_BFS_CRES Works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Project schedule is extended </t>
+  </si>
+  <si>
+    <t>Tableau Desktop and Server Environment was purchased</t>
+  </si>
+  <si>
+    <t>31/05/2016</t>
+  </si>
+  <si>
+    <t>Workspace Utilization</t>
+  </si>
+  <si>
+    <t>CRES Offering Status Report -May 2016</t>
+  </si>
+  <si>
+    <t>Santhakumar</t>
+  </si>
+  <si>
+    <t>PHI is 91.5</t>
+  </si>
+  <si>
+    <t>Target &lt;100&gt;, Actuals &lt;91.5&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Plan for next month&gt; Big Data Integration, Facility Management Dashboard</t>
+  </si>
+  <si>
+    <t>Sivaranjan</t>
+  </si>
+  <si>
+    <t>10th March 2016</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lease and Rental payment module development -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Creation of Dashbaord to capture rental and Lease payment details by floor, building, City and Region against Market Price</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lease and Rental payment module development CHANGES -
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sprint changes incorporated</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Energy Consumption module development
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actual Energy consumes vs Budget energy Consumption</t>
+    </r>
+  </si>
+  <si>
+    <t>CRES Service Offering is a solution to measure  the utilization of seats, meeting room, board room facilities, Lease, Rent and Engery Utilization in percentage and actual currency
 1) Accurately captures the seats utilised BU/floor/duilding/site/location/country/region wise.
+1) Accurately captures the Lease, Rent and Engery utilised in  BU/floor/duilding/site/location/country/region wise.
 2) Utilization of seats can be compared with the previous period.
 3) User level access screen like Executive and Admin Dashboard.</t>
   </si>
   <si>
-    <t>PRJ-4660 - OEG_BFS_CRES Works</t>
+    <t>Not Needed</t>
+  </si>
+  <si>
+    <t>No risk</t>
+  </si>
+  <si>
+    <t>No Risk</t>
+  </si>
+  <si>
+    <t>&lt;mention the pending needs and challenges if any&gt;  No pending task</t>
+  </si>
+  <si>
+    <t>&lt;Refer critical risks from PP&gt;  No Risk</t>
+  </si>
+  <si>
+    <t>&lt;Refer critical issues from PP / WSR&gt; No Risk</t>
+  </si>
+  <si>
+    <t>Review by Competency  - completed on 31-5-2016</t>
+  </si>
+  <si>
+    <t>Open NC / Observations of IQA  : No Open NC</t>
+  </si>
+  <si>
+    <t>No issues</t>
+  </si>
+  <si>
+    <t>Severity  : none</t>
   </si>
   <si>
     <r>
@@ -282,8 +366,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Accomplished:
-</t>
+      <t>Accomplished:
+Lease and Rental Payment Module:</t>
     </r>
     <r>
       <rPr>
@@ -294,30 +378,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Executive</t>
+      <t xml:space="preserve">
+1. Creation of Dashbaord to capture rental and Lease payment details by floor, building, City and Region against Market Price - </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Dashboard completed </t>
-    </r>
-    <r>
-      <rPr>
+        <i/>
         <sz val="11"/>
         <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t>Completed</t>
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -325,8 +402,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Allocation completed in Executive Dashboard 
-Admin Console Completed
 </t>
     </r>
     <r>
@@ -339,11 +414,34 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Challenges:
-</t>
+      <t>Energy Consumption Module:</t>
     </r>
     <r>
       <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.Creation of Dashbaord to capture Actual Energy consumption details by floor, building, City and Region wise against Budgeted Energy Consumption - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Completed</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -353,30 +451,19 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">The Project schedule is extended </t>
-  </si>
-  <si>
-    <t>Tableau Desktop and Server Environment was purchased</t>
-  </si>
-  <si>
-    <t>lease and Rental payment module development</t>
-  </si>
-  <si>
-    <t>Lease and Rental payment module development CHANGES</t>
-  </si>
-  <si>
-    <t>31/05/2016</t>
-  </si>
-  <si>
-    <t>Energy Consumption module development</t>
-  </si>
-  <si>
-    <t>Workspace Utilization</t>
-  </si>
-  <si>
-    <t>CRES Offering Status Report -May 2016</t>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Challenges:
+NA</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -386,7 +473,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,8 +536,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -458,13 +554,13 @@
     <font>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,12 +599,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -520,7 +610,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="63">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -667,9 +757,11 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -678,39 +770,13 @@
         <color theme="0"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="0"/>
       </right>
       <top style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -814,26 +880,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1117,17 +1163,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color theme="0"/>
       </top>
@@ -1278,6 +1313,96 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1287,274 +1412,291 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1986,12 +2128,12 @@
         <c:gapWidth val="55"/>
         <c:gapDepth val="55"/>
         <c:shape val="pyramid"/>
-        <c:axId val="200976640"/>
-        <c:axId val="201081216"/>
+        <c:axId val="103937152"/>
+        <c:axId val="103938688"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="200976640"/>
+        <c:axId val="103937152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2001,7 +2143,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201081216"/>
+        <c:crossAx val="103938688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2009,7 +2151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201081216"/>
+        <c:axId val="103938688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2019,7 +2161,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200976640"/>
+        <c:crossAx val="103937152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2504,12 +2646,12 @@
         <c:gapWidth val="55"/>
         <c:gapDepth val="55"/>
         <c:shape val="pyramid"/>
-        <c:axId val="190021632"/>
-        <c:axId val="190023168"/>
+        <c:axId val="104288640"/>
+        <c:axId val="104290176"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="190021632"/>
+        <c:axId val="104288640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2519,7 +2661,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190023168"/>
+        <c:crossAx val="104290176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2527,7 +2669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190023168"/>
+        <c:axId val="104290176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2537,7 +2679,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190021632"/>
+        <c:crossAx val="104288640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2710,40 +2852,40 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Mohamed younus A" refreshedDate="42450.750070833332" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="17">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Sivaranjan S" refreshedDate="42527.69999641204" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="14">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A2:H31" sheet="ConsultantMatrix"/>
+    <worksheetSource ref="A2:H16" sheet="ConsultantMatrix"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Name" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Role" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Grade" numFmtId="0">
       <sharedItems containsBlank="1" count="8">
-        <s v="G3"/>
-        <s v="G2"/>
         <s v="G5"/>
-        <s v="G6"/>
-        <s v="G7"/>
-        <s v="G8"/>
-        <s v="G4"/>
         <m/>
+        <s v="G2" u="1"/>
+        <s v="G4" u="1"/>
+        <s v="G6" u="1"/>
+        <s v="G8" u="1"/>
+        <s v="G3" u="1"/>
+        <s v="G7" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="% Allocated" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="100" maxValue="100"/>
     </cacheField>
     <cacheField name="Consultant Start Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Consultant Release Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-09-01T00:00:00" maxDate="2016-09-02T00:00:00"/>
     </cacheField>
     <cacheField name="Owning Unit" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Remarks" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
@@ -2758,31 +2900,31 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="17">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="14">
   <r>
-    <m/>
-    <m/>
+    <s v="Santhakumar"/>
+    <s v="PM"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <n v="100"/>
+    <s v="10th March 2016"/>
+    <d v="2016-09-01T00:00:00"/>
+    <s v="BFS"/>
     <m/>
   </r>
   <r>
-    <m/>
-    <m/>
+    <s v="Sivaranjan"/>
+    <s v="Developer"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <n v="100"/>
+    <s v="10th March 2016"/>
+    <d v="2016-09-01T00:00:00"/>
+    <s v="BFS"/>
     <m/>
   </r>
   <r>
     <m/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2792,7 +2934,7 @@
   <r>
     <m/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2802,7 +2944,7 @@
   <r>
     <m/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2812,7 +2954,7 @@
   <r>
     <m/>
     <m/>
-    <x v="0"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2832,7 +2974,7 @@
   <r>
     <m/>
     <m/>
-    <x v="2"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2842,7 +2984,7 @@
   <r>
     <m/>
     <m/>
-    <x v="3"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2852,7 +2994,7 @@
   <r>
     <m/>
     <m/>
-    <x v="3"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2862,7 +3004,7 @@
   <r>
     <m/>
     <m/>
-    <x v="4"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2872,7 +3014,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2882,7 +3024,7 @@
   <r>
     <m/>
     <m/>
-    <x v="5"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2892,37 +3034,7 @@
   <r>
     <m/>
     <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="6"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="7"/>
+    <x v="1"/>
     <m/>
     <m/>
     <m/>
@@ -2934,20 +3046,20 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:A5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="9">
-        <item x="1"/>
+        <item m="1" x="2"/>
+        <item m="1" x="6"/>
         <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item h="1" x="7"/>
-        <item x="5"/>
-        <item x="6"/>
+        <item m="1" x="4"/>
+        <item m="1" x="7"/>
+        <item h="1" x="1"/>
+        <item m="1" x="5"/>
+        <item m="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2960,27 +3072,9 @@
   <rowFields count="1">
     <field x="2"/>
   </rowFields>
-  <rowItems count="8">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
+  <rowItems count="2">
     <i>
       <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
     </i>
     <i t="grand">
       <x/>
@@ -2989,9 +3083,6 @@
   <colItems count="1">
     <i/>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Grade" fld="2" subtotal="count" baseField="0" baseItem="2683416"/>
-  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3290,8 +3381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:I57"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3305,733 +3396,761 @@
   <sheetData>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="91" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="93"/>
+      <c r="B4" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="59"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="13"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="112"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="80"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="112"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="80"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>79</v>
+      <c r="C8" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="111"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="112"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="80"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="24" t="s">
-        <v>76</v>
+      <c r="C9" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="112"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="80"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="18" t="s">
+        <v>71</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="111"/>
-      <c r="H10" s="111"/>
-      <c r="I10" s="112"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="80"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>89</v>
+      <c r="C11" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="112"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="80"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>78</v>
+      <c r="C12" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="112"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="46">
+      <c r="B13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="38">
         <v>42439</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="35"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="47">
-        <v>42551</v>
+      <c r="B14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="39">
+        <v>42643</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="35"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="45"/>
+      <c r="C15" s="37">
+        <v>92524</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="35"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="28"/>
     </row>
     <row r="16" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="113" t="s">
+      <c r="B17" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="114"/>
-      <c r="D17" s="114"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="114"/>
-      <c r="G17" s="114"/>
-      <c r="H17" s="114"/>
-      <c r="I17" s="115"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="83"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="108"/>
-      <c r="D18" s="108"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="108"/>
-      <c r="G18" s="108"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="109"/>
+      <c r="B18" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="77"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="110"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="109"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="77"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="110"/>
-      <c r="C20" s="108"/>
-      <c r="D20" s="108"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="108"/>
-      <c r="G20" s="108"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="109"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="77"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="110"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="109"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="110"/>
-      <c r="C22" s="108"/>
-      <c r="D22" s="108"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="108"/>
-      <c r="G22" s="108"/>
-      <c r="H22" s="108"/>
-      <c r="I22" s="109"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="77"/>
+    </row>
+    <row r="22" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="78"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="77"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="13"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="57"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="98"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="60"/>
+      <c r="B25" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="101"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="61"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="63"/>
+      <c r="B26" s="102"/>
+      <c r="C26" s="103"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="103"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="103"/>
+      <c r="I26" s="104"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="61"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="63"/>
+      <c r="B27" s="102"/>
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="103"/>
+      <c r="I27" s="104"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="63"/>
+      <c r="B28" s="102"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="104"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="61"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="63"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="61"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="63"/>
-    </row>
-    <row r="31" spans="2:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="61"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="63"/>
+      <c r="B29" s="102"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="103"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="103"/>
+      <c r="G29" s="103"/>
+      <c r="H29" s="103"/>
+      <c r="I29" s="104"/>
+    </row>
+    <row r="30" spans="2:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="102"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="104"/>
+    </row>
+    <row r="31" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="102"/>
+      <c r="C31" s="103"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="103"/>
+      <c r="I31" s="104"/>
     </row>
     <row r="32" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="61"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="63"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="104"/>
     </row>
     <row r="33" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="64"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="66"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="106"/>
+      <c r="I33" s="107"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="13"/>
+      <c r="I34" s="9"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="54"/>
+      <c r="B35" s="93" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="95"/>
     </row>
     <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="71"/>
+    </row>
+    <row r="37" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="103" t="s">
+      <c r="C37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="74"/>
+    </row>
+    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="104"/>
-    </row>
-    <row r="37" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="16" t="s">
+      <c r="C38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="71"/>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="74"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="105" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="85"/>
-      <c r="F37" s="85"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="106"/>
-    </row>
-    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="103" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="104"/>
-    </row>
-    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="105"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="106"/>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="103" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="99"/>
-      <c r="F40" s="99"/>
-      <c r="G40" s="99"/>
-      <c r="H40" s="99"/>
-      <c r="I40" s="104"/>
+      <c r="D40" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="71"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="16" t="s">
-        <v>22</v>
+      <c r="B41" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="105"/>
-      <c r="E41" s="85"/>
-      <c r="F41" s="85"/>
-      <c r="G41" s="85"/>
-      <c r="H41" s="85"/>
-      <c r="I41" s="106"/>
+        <v>73</v>
+      </c>
+      <c r="D41" s="72"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="74"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="103" t="s">
-        <v>26</v>
-      </c>
-      <c r="E42" s="99"/>
-      <c r="F42" s="99"/>
-      <c r="G42" s="99"/>
-      <c r="H42" s="99"/>
-      <c r="I42" s="104"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="12"/>
+      <c r="B42" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="56">
+        <v>0</v>
+      </c>
+      <c r="D42" s="70"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="71"/>
+    </row>
+    <row r="43" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="8"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
-      <c r="I43" s="13"/>
+      <c r="I43" s="9"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="101" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="95"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="102"/>
-      <c r="G44" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="71"/>
-      <c r="G45" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="H45" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="I45" s="18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="H46" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="I46" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="73"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="H47" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="I47" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="72"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="19"/>
+      <c r="B44" s="68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="108" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="109"/>
+      <c r="D45" s="109"/>
+      <c r="E45" s="109"/>
+      <c r="F45" s="109"/>
+      <c r="G45" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="H45" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" s="53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="110" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="111"/>
+      <c r="D46" s="111"/>
+      <c r="E46" s="111"/>
+      <c r="F46" s="111"/>
+      <c r="G46" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I46" s="53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="109"/>
+      <c r="D47" s="109"/>
+      <c r="E47" s="109"/>
+      <c r="F47" s="109"/>
+      <c r="G47" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="H47" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I47" s="53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="118"/>
+      <c r="C48" s="119"/>
+      <c r="D48" s="119"/>
+      <c r="E48" s="119"/>
+      <c r="F48" s="119"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="55"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="12"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
-      <c r="I49" s="13"/>
+      <c r="I49" s="9"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="90" t="s">
+      <c r="B50" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="67"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="62"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" s="25"/>
+      <c r="E51" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="64"/>
+      <c r="G51" s="120">
+        <v>0</v>
+      </c>
+      <c r="H51" s="121"/>
+      <c r="I51" s="122"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="25"/>
+      <c r="E52" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" s="19"/>
+      <c r="G52" s="112">
+        <v>100</v>
+      </c>
+      <c r="H52" s="113"/>
+      <c r="I52" s="114"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" s="25"/>
+      <c r="E53" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53" s="65"/>
+      <c r="G53" s="115">
+        <v>100</v>
+      </c>
+      <c r="H53" s="116"/>
+      <c r="I53" s="117"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="25"/>
+      <c r="E54" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" s="91"/>
+      <c r="G54" s="91"/>
+      <c r="H54" s="91"/>
+      <c r="I54" s="92"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="8"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="100"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="94" t="s">
-        <v>38</v>
-      </c>
-      <c r="F50" s="95"/>
-      <c r="G50" s="95"/>
-      <c r="H50" s="95"/>
-      <c r="I50" s="96"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
+      <c r="G55" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I55" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C51" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D51" s="32"/>
-      <c r="E51" s="97" t="s">
-        <v>39</v>
-      </c>
-      <c r="F51" s="98"/>
-      <c r="G51" s="80"/>
-      <c r="H51" s="81"/>
-      <c r="I51" s="82"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="32"/>
-      <c r="E52" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="26"/>
-      <c r="G52" s="76"/>
-      <c r="H52" s="73"/>
-      <c r="I52" s="77"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="51"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="99" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" s="99"/>
-      <c r="G53" s="78"/>
-      <c r="H53" s="70"/>
-      <c r="I53" s="79"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="F54" s="67"/>
-      <c r="G54" s="67"/>
-      <c r="H54" s="67"/>
-      <c r="I54" s="68"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="12"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G55" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I55" s="20" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="12"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="29"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="22"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="90" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="67"/>
-      <c r="D57" s="67"/>
-      <c r="E57" s="67"/>
-      <c r="F57" s="67"/>
-      <c r="G57" s="67"/>
-      <c r="H57" s="67"/>
-      <c r="I57" s="68"/>
+      <c r="B57" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="91"/>
+      <c r="D57" s="91"/>
+      <c r="E57" s="91"/>
+      <c r="F57" s="91"/>
+      <c r="G57" s="91"/>
+      <c r="H57" s="91"/>
+      <c r="I57" s="92"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="87" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C58" s="88"/>
-      <c r="D58" s="75" t="s">
-        <v>84</v>
-      </c>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
-      <c r="I58" s="89"/>
+      <c r="D58" s="89" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" s="89"/>
+      <c r="F58" s="89"/>
+      <c r="G58" s="89"/>
+      <c r="H58" s="89"/>
+      <c r="I58" s="90"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="C59" s="84"/>
-      <c r="D59" s="85"/>
-      <c r="E59" s="85"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="85"/>
-      <c r="H59" s="85"/>
+      <c r="B59" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="85"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="73"/>
       <c r="I59" s="86"/>
     </row>
     <row r="60" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="21"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="23"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:I33"/>
+    <mergeCell ref="E54:I54"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:I59"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:I58"/>
+    <mergeCell ref="B57:I57"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="E50:I50"/>
     <mergeCell ref="E51:F51"/>
@@ -4048,22 +4167,6 @@
     <mergeCell ref="G6:I12"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="D39:I39"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:I59"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:I58"/>
-    <mergeCell ref="B57:I57"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B25:I33"/>
-    <mergeCell ref="E54:I54"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="G51:I51"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
@@ -4078,141 +4181,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.140625" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="116" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="123" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
+      <c r="D3" s="40">
+        <v>100</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="41">
+        <v>42614</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
+      <c r="A4" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="40">
+        <v>100</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="41">
+        <v>42614</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="49"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
+      <c r="A5" s="42"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="43"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="44"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4227,7 +4321,7 @@
   <dimension ref="A3:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4238,166 +4332,121 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>72</v>
+      <c r="A3" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="36">
-        <v>1</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="41">
+      <c r="A4" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="33">
         <v>0</v>
       </c>
-      <c r="G4" s="42">
+      <c r="G4" s="34">
         <f>F4/(SUM($F$4:$F$12))</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="36">
-        <v>6</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="41">
+      <c r="A5" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="33">
         <v>0</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="34">
         <f t="shared" ref="G5:G11" si="0">F5/(SUM($F$4:$F$12))</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="36">
-        <v>1</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="41">
+      <c r="E6" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="33">
         <v>0</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="36">
+      <c r="E7" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="33">
         <v>2</v>
       </c>
-      <c r="E7" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="41">
-        <v>2</v>
-      </c>
-      <c r="G7" s="42">
+      <c r="G7" s="34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="36">
-        <v>1</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="41">
+      <c r="E8" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="33">
         <v>0</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="36">
-        <v>2</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="41">
+      <c r="E9" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="33">
         <v>0</v>
       </c>
-      <c r="G9" s="42">
+      <c r="G9" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="36">
-        <v>3</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="41">
+      <c r="E10" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="33">
         <v>0</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="36">
-        <v>16</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42">
+      <c r="E11" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="40"/>
+      <c r="E12" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>